<commit_message>
added my parts, this is the main tex file again
</commit_message>
<xml_diff>
--- a/marktanteile.xlsx
+++ b/marktanteile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (5)" sheetId="6" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="22">
   <si>
     <t>Toyota Motor Corporation</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Suzuki</t>
+  </si>
+  <si>
+    <t>Hyundai</t>
   </si>
 </sst>
 </file>
@@ -192,7 +195,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -753,9 +755,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -965,7 +965,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1239,7 +1238,6 @@
                     <a:noFill/>
                   </a:ln>
                 </c15:spPr>
-                <c15:layout/>
               </c:ext>
             </c:extLst>
           </c:dLbls>
@@ -1809,7 +1807,6 @@
                     <a:noFill/>
                   </a:ln>
                 </c15:spPr>
-                <c15:layout/>
               </c:ext>
             </c:extLst>
           </c:dLbls>
@@ -2787,9 +2784,8 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="20000"/>
-                  <a:lumOff val="80000"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln w="19050">
@@ -2854,54 +2850,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="b" anchorCtr="0">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1"/>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:prstGeom prst="rect">
-                      <a:avLst/>
-                    </a:prstGeom>
-                    <a:noFill/>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                  </c15:spPr>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="6"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -3016,16 +2964,16 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Fiat</c:v>
+                  <c:v>Hyundai</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>BMW Group</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>General Motors</c:v>
+                  <c:v>Fiat</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>BMW Group</c:v>
+                  <c:v>Nissan Motor Corporation</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Ford Motor Company</c:v>
@@ -3034,7 +2982,7 @@
                   <c:v>Daimler</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Nissan Motor Corporation</c:v>
+                  <c:v>General Motors</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Toyota</c:v>
@@ -3055,16 +3003,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>5.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.9</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>9</c:v>
@@ -3073,7 +3021,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>12</c:v>
@@ -3229,7 +3177,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3604,7 +3551,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3881,7 +3827,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9319,7 +9264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
@@ -9408,18 +9353,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:D11"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="3" spans="3:4" x14ac:dyDescent="0.25">
@@ -9432,18 +9377,18 @@
     </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D4">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>5.9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.25">
@@ -9464,10 +9409,10 @@
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.25">

</xml_diff>